<commit_message>
Allow pdf output to use extracted report type and notes
</commit_message>
<xml_diff>
--- a/quarterlyReports/pchs_report_format.xlsx
+++ b/quarterlyReports/pchs_report_format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mayalapp/Documents/coding_projects/dad_data_project/quarterlyReports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8D6AA7-0A8C-CB46-90D5-49739D1ABD20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59691190-D77E-2643-A949-C099036A170E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24540" windowHeight="12580" tabRatio="232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24540" windowHeight="14440" tabRatio="232" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="26">
   <si>
     <t xml:space="preserve">Location: </t>
   </si>
@@ -89,15 +89,6 @@
   </si>
   <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>All patient notes here</t>
-  </si>
-  <si>
-    <t>Screened patient notes here</t>
-  </si>
-  <si>
-    <t>Name of report (e.g. "Mammogram screening")</t>
   </si>
   <si>
     <r>
@@ -148,6 +139,21 @@
       </rPr>
       <t xml:space="preserve"> QUARTER DATES HERE</t>
     </r>
+  </si>
+  <si>
+    <t>Patients meeting criteria</t>
+  </si>
+  <si>
+    <t>Patients not meeting criteria</t>
+  </si>
+  <si>
+    <t>Notes describing criteria for patients</t>
+  </si>
+  <si>
+    <t>Notes describing total patients</t>
+  </si>
+  <si>
+    <t>Name of report type (e.g. "Mammogram screening")</t>
   </si>
 </sst>
 </file>
@@ -713,13 +719,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{432A7C2E-DA82-8540-BAE9-3AF55A86A91F}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="34.5" style="4" customWidth="1"/>
+    <col min="1" max="1" width="40.25" style="4" customWidth="1"/>
     <col min="2" max="16384" width="10.75" style="4"/>
   </cols>
   <sheetData>
@@ -728,7 +734,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -739,7 +745,7 @@
         <v>18</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -748,7 +754,7 @@
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="13"/>
       <c r="B3" s="12" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -763,7 +769,7 @@
     </row>
     <row r="5" spans="1:19" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -946,7 +952,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>16</v>
@@ -1005,7 +1011,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>16</v>
@@ -1086,7 +1092,7 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A17" s="9" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>16</v>
@@ -1097,7 +1103,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A18" s="9" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>16</v>
@@ -1108,7 +1114,7 @@
     </row>
     <row r="21" spans="1:19" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1291,7 +1297,7 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A26" s="9" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>16</v>
@@ -1350,7 +1356,7 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A27" s="9" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>16</v>
@@ -1480,13 +1486,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14D2DAAB-C54B-B648-806A-56E55F9E768F}">
   <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="33.25" style="4" customWidth="1"/>
+    <col min="1" max="1" width="40" style="4" customWidth="1"/>
     <col min="2" max="16384" width="10.75" style="4"/>
   </cols>
   <sheetData>
@@ -1495,7 +1501,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -1506,7 +1512,7 @@
         <v>18</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -1515,7 +1521,7 @@
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="13"/>
       <c r="B3" s="12" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -1530,7 +1536,7 @@
     </row>
     <row r="5" spans="1:19" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1713,7 +1719,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>16</v>
@@ -1772,7 +1778,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>16</v>
@@ -1853,7 +1859,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="9" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>16</v>
@@ -1864,7 +1870,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="9" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>16</v>

</xml_diff>